<commit_message>
Added formatting & restrictions to results spreadsheet & added results tables to report
</commit_message>
<xml_diff>
--- a/assignment2/data/results/summary.xlsx
+++ b/assignment2/data/results/summary.xlsx
@@ -16,6 +16,7 @@
     <sheet name="nb-defaultsort" sheetId="10" r:id="rId7"/>
     <sheet name="nb-cssort" sheetId="11" r:id="rId8"/>
     <sheet name="nb-scsort" sheetId="12" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -23,15 +24,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="22">
-  <si>
-    <t>Correctly Classified</t>
-  </si>
-  <si>
-    <t>Mean absolute error</t>
-  </si>
-  <si>
-    <t>Root mean squared error</t>
-  </si>
   <si>
     <t>Weighted Avg. Precision</t>
   </si>
@@ -72,9 +64,6 @@
     <t xml:space="preserve">   testing/9</t>
   </si>
   <si>
-    <t>10 sets of 5000 (avg)</t>
-  </si>
-  <si>
     <t>Ratio Subsets (avg)</t>
   </si>
   <si>
@@ -87,14 +76,29 @@
     <t xml:space="preserve">   training/2</t>
   </si>
   <si>
-    <t>initial 10-fold crossv</t>
+    <t>10-fold crossv</t>
+  </si>
+  <si>
+    <t>RMS error</t>
+  </si>
+  <si>
+    <t>Mean Abs. error</t>
+  </si>
+  <si>
+    <t>Correct Class. %</t>
+  </si>
+  <si>
+    <t>Test sets (avg)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,23 +122,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,16 +139,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,73 +479,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="7">
+        <v>57.536999999999999</v>
+      </c>
+      <c r="C2" s="7">
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.24629999999999999</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.57499999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>57.536999999999999</v>
-      </c>
-      <c r="C2">
-        <v>9.8599999999999993E-2</v>
-      </c>
-      <c r="D2">
-        <v>0.24629999999999999</v>
-      </c>
-      <c r="E2">
-        <v>0.53700000000000003</v>
-      </c>
-      <c r="F2">
-        <v>0.57499999999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <f>AVERAGE(B5:B14)</f>
         <v>57.716000000000008</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:F4" si="0">AVERAGE(C5:C14)</f>
         <v>9.8659999999999998E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>0.24587000000000003</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>0.53980000000000017</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>0.57709999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>57.06</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>59.22</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>57.14</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>57.34</v>
@@ -625,7 +625,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>58.82</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>58.24</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>57.38</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>57.68</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>57.68</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>56.6</v>
@@ -744,33 +744,33 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
         <v>71.815399999999997</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
         <v>7.5600000000000001E-2</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <f t="shared" si="1"/>
         <v>0.19443333333333332</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0.72733333333333328</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>0.71799999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>71.508600000000001</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>72.809100000000001</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>71.128500000000003</v>
@@ -831,6 +831,20 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -839,7 +853,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F16" sqref="B16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,73 +866,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6">
+        <v>93.602599999999995</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.10970000000000001</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>93.602599999999995</v>
-      </c>
-      <c r="C2">
-        <v>2.1499999999999998E-2</v>
-      </c>
-      <c r="D2">
-        <v>0.10970000000000001</v>
-      </c>
-      <c r="E2">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="F2">
-        <v>0.93600000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <f>AVERAGE(B5:B14)</f>
         <v>94</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:F4" si="0">AVERAGE(C5:C14)</f>
         <v>2.0190000000000003E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>0.10645000000000002</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>0.93769999999999987</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>0.93979999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>93.92</v>
@@ -938,7 +952,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>94.14</v>
@@ -958,7 +972,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>94.54</v>
@@ -978,7 +992,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>93.74</v>
@@ -998,7 +1012,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>94.02</v>
@@ -1018,7 +1032,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>93.88</v>
@@ -1038,7 +1052,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>94.44</v>
@@ -1058,7 +1072,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>94.08</v>
@@ -1078,7 +1092,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>93.3</v>
@@ -1098,7 +1112,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>93.94</v>
@@ -1117,33 +1131,33 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
         <v>95.191400000000002</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
         <v>1.7366666666666666E-2</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <f t="shared" si="1"/>
         <v>9.3699999999999992E-2</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0.94999999999999984</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>95.097999999999999</v>
@@ -1163,7 +1177,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>94.998000000000005</v>
@@ -1183,7 +1197,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>95.478200000000001</v>
@@ -1212,7 +1226,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B16" sqref="B16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,73 +1239,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6">
+        <v>55.989600000000003</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.1057</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.2319</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>55.989600000000003</v>
-      </c>
-      <c r="C2">
-        <v>0.1057</v>
-      </c>
-      <c r="D2">
-        <v>0.2319</v>
-      </c>
-      <c r="E2">
-        <v>0.53200000000000003</v>
-      </c>
-      <c r="F2">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <f>AVERAGE(B5:B14)</f>
         <v>56.398000000000003</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:F4" si="0">AVERAGE(C5:C14)</f>
         <v>0.10491000000000002</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>0.23126000000000002</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>0.53279999999999994</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>0.56399999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>54.86</v>
@@ -1311,7 +1325,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>57.62</v>
@@ -1331,7 +1345,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>55.64</v>
@@ -1351,7 +1365,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>56.3</v>
@@ -1371,7 +1385,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>57.08</v>
@@ -1391,7 +1405,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>56.04</v>
@@ -1411,7 +1425,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>55.82</v>
@@ -1431,7 +1445,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>56.26</v>
@@ -1451,7 +1465,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>56.96</v>
@@ -1471,7 +1485,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>57.4</v>
@@ -1490,33 +1504,33 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
         <v>58.169900000000005</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
         <v>0.10276666666666666</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <f t="shared" si="1"/>
         <v>0.22670000000000001</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0.56300000000000006</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>0.58166666666666667</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>57.763100000000001</v>
@@ -1536,7 +1550,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>58.623399999999997</v>
@@ -1556,7 +1570,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>58.123199999999997</v>
@@ -1585,7 +1599,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F19" sqref="A1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,73 +1612,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6">
+        <v>93.426599999999993</v>
+      </c>
+      <c r="C2" s="6">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="D2" s="6">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>93.426599999999993</v>
-      </c>
-      <c r="C2">
-        <v>9.7999999999999997E-3</v>
-      </c>
-      <c r="D2">
-        <v>7.4700000000000003E-2</v>
-      </c>
-      <c r="E2">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="F2">
-        <v>0.93400000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <f>AVERAGE(B5:B14)</f>
         <v>94.36</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:F4" si="0">AVERAGE(C5:C14)</f>
         <v>7.9600000000000001E-3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>6.2869999999999995E-2</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>0.89900000000000002</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>0.94349999999999989</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>93.68</v>
@@ -1684,7 +1698,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>94.54</v>
@@ -1704,7 +1718,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>94.58</v>
@@ -1724,7 +1738,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>94.94</v>
@@ -1744,7 +1758,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>94.58</v>
@@ -1764,7 +1778,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>94.52</v>
@@ -1784,7 +1798,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>94.64</v>
@@ -1804,7 +1818,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>94.24</v>
@@ -1824,7 +1838,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>94.16</v>
@@ -1844,7 +1858,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>93.72</v>
@@ -1863,33 +1877,33 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
         <v>94.804599999999994</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
         <v>6.8333333333333336E-3</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <f t="shared" si="1"/>
         <v>5.5766666666666666E-2</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0.90300000000000002</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>0.94799999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>94.797899999999998</v>
@@ -1909,7 +1923,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>94.737899999999996</v>
@@ -1929,7 +1943,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>94.878</v>
@@ -1958,7 +1972,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,73 +1985,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6">
+        <v>94.422200000000004</v>
+      </c>
+      <c r="C2" s="6">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="D2" s="6">
+        <v>6.3299999999999995E-2</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.94399999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>94.422200000000004</v>
-      </c>
-      <c r="C2">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="D2">
-        <v>6.3299999999999995E-2</v>
-      </c>
-      <c r="E2">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="F2">
-        <v>0.94399999999999995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <f>AVERAGE(B5:B14)</f>
         <v>94.318000000000012</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:F4" si="0">AVERAGE(C5:C14)</f>
         <v>7.3099999999999997E-3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>6.3E-2</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>0.89790000000000014</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>0.94309999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>94.7</v>
@@ -2057,7 +2071,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>94.44</v>
@@ -2077,7 +2091,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>93.88</v>
@@ -2097,7 +2111,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>94.8</v>
@@ -2117,7 +2131,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>94.5</v>
@@ -2137,7 +2151,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>94.24</v>
@@ -2157,7 +2171,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>94.7</v>
@@ -2177,7 +2191,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>94.22</v>
@@ -2197,7 +2211,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>93.74</v>
@@ -2217,7 +2231,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>93.96</v>
@@ -2236,33 +2250,33 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
         <v>94.644533333333342</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
         <v>6.4666666666666666E-3</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <f t="shared" si="1"/>
         <v>5.7666666666666665E-2</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0.90166666666666673</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>0.94666666666666666</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>94.677899999999994</v>
@@ -2282,7 +2296,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>94.797899999999998</v>
@@ -2302,7 +2316,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>94.457800000000006</v>
@@ -2331,7 +2345,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F16" sqref="B16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,73 +2358,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6">
+        <v>88.752499999999998</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2.01E-2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.11840000000000001</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.879</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>88.752499999999998</v>
-      </c>
-      <c r="C2">
-        <v>2.01E-2</v>
-      </c>
-      <c r="D2">
-        <v>0.11840000000000001</v>
-      </c>
-      <c r="E2">
-        <v>0.879</v>
-      </c>
-      <c r="F2">
-        <v>0.88800000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <f>AVERAGE(B5:B14)</f>
         <v>86.713999999999999</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <f t="shared" ref="C4:F4" si="0">AVERAGE(C5:C14)</f>
         <v>2.4419999999999997E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <f t="shared" si="0"/>
         <v>0.13320000000000001</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>0.86490000000000011</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <f t="shared" si="0"/>
         <v>0.86729999999999985</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>85.46</v>
@@ -2430,7 +2444,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>87.64</v>
@@ -2450,7 +2464,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>87.06</v>
@@ -2470,7 +2484,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>86.66</v>
@@ -2490,7 +2504,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>86.48</v>
@@ -2510,7 +2524,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>86.32</v>
@@ -2530,7 +2544,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>86.18</v>
@@ -2550,7 +2564,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>86.6</v>
@@ -2570,7 +2584,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>87.26</v>
@@ -2590,7 +2604,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>87.48</v>
@@ -2609,33 +2623,33 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="8">
         <f>AVERAGE(B17:B19)</f>
         <v>88.82886666666667</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="8">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
         <v>2.0166666666666666E-2</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="8">
         <f t="shared" si="1"/>
         <v>0.11766666666666666</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="8">
         <f t="shared" si="1"/>
         <v>0.88566666666666671</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="8">
         <f t="shared" si="1"/>
         <v>0.88833333333333331</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>88.775499999999994</v>
@@ -2655,7 +2669,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>88.8155</v>
@@ -2675,7 +2689,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>88.895600000000002</v>
@@ -2704,7 +2718,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection sqref="A1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2717,73 +2731,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6">
+        <v>49.064399999999999</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.11360000000000001</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.2387</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>49.064399999999999</v>
-      </c>
-      <c r="C2">
-        <v>0.11360000000000001</v>
-      </c>
-      <c r="D2">
-        <v>0.2387</v>
-      </c>
-      <c r="E2">
-        <v>0.42099999999999999</v>
-      </c>
-      <c r="F2">
-        <v>0.49099999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <f>AVERAGE(B5:B14)</f>
         <v>49.236000000000004</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:F4" si="0">AVERAGE(C5:C14)</f>
         <v>0.11351000000000003</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>0.23844999999999997</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>0.42259999999999998</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>0.49230000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>49.14</v>
@@ -2803,7 +2817,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>50.16</v>
@@ -2823,7 +2837,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>48.18</v>
@@ -2843,7 +2857,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>49.24</v>
@@ -2863,7 +2877,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>48.66</v>
@@ -2883,7 +2897,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>49.72</v>
@@ -2903,7 +2917,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>48.84</v>
@@ -2923,7 +2937,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>49.84</v>
@@ -2943,7 +2957,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>49.52</v>
@@ -2963,7 +2977,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>49.06</v>
@@ -2982,33 +2996,33 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
         <v>49.986666666666672</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
         <v>0.11326666666666667</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <f t="shared" si="1"/>
         <v>0.23796666666666666</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0.44933333333333336</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>50.420200000000001</v>
@@ -3028,7 +3042,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>49.859900000000003</v>
@@ -3048,7 +3062,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>49.679900000000004</v>
@@ -3077,7 +3091,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F16" sqref="B16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3090,73 +3104,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6">
+        <v>62.7149</v>
+      </c>
+      <c r="C2" s="6">
+        <v>9.2200000000000004E-2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.21740000000000001</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>62.7149</v>
-      </c>
-      <c r="C2">
-        <v>9.2200000000000004E-2</v>
-      </c>
-      <c r="D2">
-        <v>0.21740000000000001</v>
-      </c>
-      <c r="E2">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="F2">
-        <v>0.627</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <f>AVERAGE(B5:B14)</f>
         <v>62.311999999999991</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:F4" si="0">AVERAGE(C5:C14)</f>
         <v>9.2659999999999992E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>0.21825999999999998</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>0.61370000000000002</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>0.62309999999999988</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>63.18</v>
@@ -3176,7 +3190,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>63.3</v>
@@ -3196,7 +3210,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>63.42</v>
@@ -3216,7 +3230,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>61.6</v>
@@ -3236,7 +3250,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>62.22</v>
@@ -3256,7 +3270,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>62.14</v>
@@ -3276,7 +3290,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>61.58</v>
@@ -3296,7 +3310,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>61.58</v>
@@ -3316,7 +3330,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>61.66</v>
@@ -3336,7 +3350,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>62.44</v>
@@ -3355,33 +3369,33 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
         <v>63.165266666666668</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
         <v>9.1766666666666663E-2</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <f t="shared" si="1"/>
         <v>0.21653333333333333</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0.628</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>0.63166666666666671</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>63.285299999999999</v>
@@ -3401,7 +3415,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>63.205300000000001</v>
@@ -3421,7 +3435,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>63.005200000000002</v>
@@ -3450,7 +3464,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B4" sqref="B4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,73 +3477,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6">
+        <v>49.380200000000002</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.1132</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.2387</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
-        <v>49.380200000000002</v>
-      </c>
-      <c r="C2">
-        <v>0.1132</v>
-      </c>
-      <c r="D2">
-        <v>0.2387</v>
-      </c>
-      <c r="E2">
-        <v>0.44600000000000001</v>
-      </c>
-      <c r="F2">
-        <v>0.49399999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <f>AVERAGE(B5:B14)</f>
         <v>49.29</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <f t="shared" ref="C4:F4" si="0">AVERAGE(C5:C14)</f>
         <v>0.11311</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>0.23849999999999999</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>0.44580000000000009</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>0.49289999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>49.48</v>
@@ -3549,7 +3563,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>49.88</v>
@@ -3569,7 +3583,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>49.9</v>
@@ -3589,7 +3603,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>49.38</v>
@@ -3609,7 +3623,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>47.96</v>
@@ -3629,7 +3643,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>49.12</v>
@@ -3649,7 +3663,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>49.24</v>
@@ -3669,7 +3683,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>48.8</v>
@@ -3689,7 +3703,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>49.4</v>
@@ -3709,7 +3723,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>49.74</v>
@@ -3728,33 +3742,33 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
         <v>50.606899999999996</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
         <v>0.11273333333333335</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <f t="shared" si="1"/>
         <v>0.23766666666666669</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0.45966666666666667</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>0.50599999999999989</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>51.320500000000003</v>
@@ -3774,7 +3788,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>49.559800000000003</v>
@@ -3794,7 +3808,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>50.940399999999997</v>

</xml_diff>

<commit_message>
Before inclusion of revised training data for NN
</commit_message>
<xml_diff>
--- a/assignment2/data/results/summary.xlsx
+++ b/assignment2/data/results/summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27645" windowHeight="12375"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="27645" windowHeight="12375" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="J48-defaultsort" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="26">
   <si>
     <t>Weighted Avg. Precision</t>
   </si>
@@ -90,13 +90,25 @@
   <si>
     <t>Test sets (avg)</t>
   </si>
+  <si>
+    <t>Unordered</t>
+  </si>
+  <si>
+    <t>By Suite</t>
+  </si>
+  <si>
+    <t>By Card Value</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -152,16 +164,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
@@ -749,23 +762,23 @@
       </c>
       <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
-        <v>71.815399999999997</v>
+        <v>51.627333333333333</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
-        <v>7.5600000000000001E-2</v>
+        <v>0.10840000000000001</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="1"/>
-        <v>0.19443333333333332</v>
+        <v>0.24786666666666668</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
-        <v>0.72733333333333328</v>
+        <v>0.47700000000000004</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>0.71799999999999997</v>
+        <v>0.51633333333333331</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -773,19 +786,19 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>71.508600000000001</v>
+        <v>52.681100000000001</v>
       </c>
       <c r="C17">
-        <v>7.5800000000000006E-2</v>
+        <v>0.1085</v>
       </c>
       <c r="D17">
-        <v>0.19450000000000001</v>
+        <v>0.24640000000000001</v>
       </c>
       <c r="E17">
-        <v>0.70899999999999996</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="F17">
-        <v>0.71499999999999997</v>
+        <v>0.52700000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -793,19 +806,19 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>72.809100000000001</v>
+        <v>51.520600000000002</v>
       </c>
       <c r="C18">
-        <v>7.46E-2</v>
+        <v>0.1081</v>
       </c>
       <c r="D18">
-        <v>0.19270000000000001</v>
+        <v>0.24790000000000001</v>
       </c>
       <c r="E18">
-        <v>0.73899999999999999</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="F18">
-        <v>0.72799999999999998</v>
+        <v>0.51500000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -813,19 +826,19 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>71.128500000000003</v>
+        <v>50.680300000000003</v>
       </c>
       <c r="C19">
-        <v>7.6399999999999996E-2</v>
+        <v>0.1086</v>
       </c>
       <c r="D19">
-        <v>0.1961</v>
+        <v>0.24929999999999999</v>
       </c>
       <c r="E19">
-        <v>0.73399999999999999</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="F19">
-        <v>0.71099999999999997</v>
+        <v>0.50700000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -836,24 +849,275 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="6">
+        <v>49.064399999999999</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.11360000000000001</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.2387</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6">
+        <v>62.7149</v>
+      </c>
+      <c r="C3" s="6">
+        <v>9.2200000000000004E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.21740000000000001</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="6">
+        <v>49.380200000000002</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.1132</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.2387</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="7">
+        <v>57.536999999999999</v>
+      </c>
+      <c r="C7" s="7">
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.24629999999999999</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.57499999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="6">
+        <v>93.602599999999995</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.10970000000000001</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6">
+        <v>55.989600000000003</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.1057</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.2319</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6">
+        <v>93.426599999999993</v>
+      </c>
+      <c r="C12" s="6">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="D12" s="6">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="6">
+        <v>94.422200000000004</v>
+      </c>
+      <c r="C13" s="6">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="D13" s="6">
+        <v>6.3299999999999995E-2</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.94399999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="6">
+        <v>88.752499999999998</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2.01E-2</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.11840000000000001</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.879</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="B16:F16"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,89 +1395,12 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4">
-        <f>AVERAGE(B17:B19)</f>
-        <v>95.191400000000002</v>
-      </c>
-      <c r="C16" s="4">
-        <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
-        <v>1.7366666666666666E-2</v>
-      </c>
-      <c r="D16" s="4">
-        <f t="shared" si="1"/>
-        <v>9.3699999999999992E-2</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.94999999999999984</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.95199999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17">
-        <v>95.097999999999999</v>
-      </c>
-      <c r="C17">
-        <v>1.7500000000000002E-2</v>
-      </c>
-      <c r="D17">
-        <v>9.4500000000000001E-2</v>
-      </c>
-      <c r="E17">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="F17">
-        <v>0.95099999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18">
-        <v>94.998000000000005</v>
-      </c>
-      <c r="C18">
-        <v>1.77E-2</v>
-      </c>
-      <c r="D18">
-        <v>9.5699999999999993E-2</v>
-      </c>
-      <c r="E18">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="F18">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19">
-        <v>95.478200000000001</v>
-      </c>
-      <c r="C19">
-        <v>1.6899999999999998E-2</v>
-      </c>
-      <c r="D19">
-        <v>9.0899999999999995E-2</v>
-      </c>
-      <c r="E19">
-        <v>0.95299999999999996</v>
-      </c>
-      <c r="F19">
-        <v>0.95499999999999996</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1226,7 +1413,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:F16"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,7 +1786,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="A1:F19"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,7 +2532,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="B16:F16"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2718,7 +2905,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F19"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3001,23 +3188,23 @@
       </c>
       <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
-        <v>49.986666666666672</v>
+        <v>47.945866666666667</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
-        <v>0.11326666666666667</v>
+        <v>0.11383333333333334</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="1"/>
-        <v>0.23796666666666666</v>
+        <v>0.24033333333333337</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
-        <v>0.44933333333333336</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.47966666666666669</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3025,19 +3212,19 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>50.420200000000001</v>
+        <v>48.679499999999997</v>
       </c>
       <c r="C17">
-        <v>0.1132</v>
+        <v>0.1137</v>
       </c>
       <c r="D17">
-        <v>0.2379</v>
+        <v>0.2402</v>
       </c>
       <c r="E17">
-        <v>0.46700000000000003</v>
+        <v>0.439</v>
       </c>
       <c r="F17">
-        <v>0.504</v>
+        <v>0.48699999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3045,19 +3232,19 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>49.859900000000003</v>
+        <v>47.258899999999997</v>
       </c>
       <c r="C18">
-        <v>0.1133</v>
+        <v>0.114</v>
       </c>
       <c r="D18">
-        <v>0.23799999999999999</v>
+        <v>0.24049999999999999</v>
       </c>
       <c r="E18">
-        <v>0.44500000000000001</v>
+        <v>0.42</v>
       </c>
       <c r="F18">
-        <v>0.499</v>
+        <v>0.47299999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3065,19 +3252,19 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>49.679900000000004</v>
+        <v>47.8992</v>
       </c>
       <c r="C19">
-        <v>0.1133</v>
+        <v>0.1138</v>
       </c>
       <c r="D19">
-        <v>0.23799999999999999</v>
+        <v>0.24030000000000001</v>
       </c>
       <c r="E19">
-        <v>0.436</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="F19">
-        <v>0.497</v>
+        <v>0.47899999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -3088,10 +3275,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="B16:F16"/>
+      <selection activeCell="F2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3369,89 +3556,12 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4">
-        <f>AVERAGE(B17:B19)</f>
-        <v>63.165266666666668</v>
-      </c>
-      <c r="C16" s="4">
-        <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
-        <v>9.1766666666666663E-2</v>
-      </c>
-      <c r="D16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.21653333333333333</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.628</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.63166666666666671</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17">
-        <v>63.285299999999999</v>
-      </c>
-      <c r="C17">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="D17">
-        <v>0.2172</v>
-      </c>
-      <c r="E17">
-        <v>0.628</v>
-      </c>
-      <c r="F17">
-        <v>0.63300000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18">
-        <v>63.205300000000001</v>
-      </c>
-      <c r="C18">
-        <v>9.1300000000000006E-2</v>
-      </c>
-      <c r="D18">
-        <v>0.2157</v>
-      </c>
-      <c r="E18">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="F18">
-        <v>0.63200000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19">
-        <v>63.005200000000002</v>
-      </c>
-      <c r="C19">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="D19">
-        <v>0.2167</v>
-      </c>
-      <c r="E19">
-        <v>0.624</v>
-      </c>
-      <c r="F19">
-        <v>0.63</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3461,10 +3571,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F4"/>
+      <selection activeCell="F2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,89 +3852,12 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4">
-        <f>AVERAGE(B17:B19)</f>
-        <v>50.606899999999996</v>
-      </c>
-      <c r="C16" s="4">
-        <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
-        <v>0.11273333333333335</v>
-      </c>
-      <c r="D16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.23766666666666669</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.45966666666666667</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.50599999999999989</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17">
-        <v>51.320500000000003</v>
-      </c>
-      <c r="C17">
-        <v>0.11260000000000001</v>
-      </c>
-      <c r="D17">
-        <v>0.23730000000000001</v>
-      </c>
-      <c r="E17">
-        <v>0.46899999999999997</v>
-      </c>
-      <c r="F17">
-        <v>0.51300000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18">
-        <v>49.559800000000003</v>
-      </c>
-      <c r="C18">
-        <v>0.113</v>
-      </c>
-      <c r="D18">
-        <v>0.23830000000000001</v>
-      </c>
-      <c r="E18">
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="F18">
-        <v>0.496</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19">
-        <v>50.940399999999997</v>
-      </c>
-      <c r="C19">
-        <v>0.11260000000000001</v>
-      </c>
-      <c r="D19">
-        <v>0.2374</v>
-      </c>
-      <c r="E19">
-        <v>0.46200000000000002</v>
-      </c>
-      <c r="F19">
-        <v>0.50900000000000001</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
All content now added to report
</commit_message>
<xml_diff>
--- a/assignment2/data/results/summary.xlsx
+++ b/assignment2/data/results/summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27645" windowHeight="12375" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="27645" windowHeight="12375" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="J48-defaultsort" sheetId="1" r:id="rId1"/>
@@ -851,7 +851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:F14"/>
     </sheetView>
   </sheetViews>
@@ -1117,7 +1117,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="F14" sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1413,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="F14" sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,7 +1786,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="F19" sqref="A1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,23 +2069,23 @@
       </c>
       <c r="B16" s="4">
         <f>AVERAGE(B17:B19)</f>
-        <v>94.804599999999994</v>
+        <v>66.820066666666662</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" ref="C16:F16" si="1">AVERAGE(C17:C19)</f>
-        <v>6.8333333333333336E-3</v>
+        <v>6.8533333333333321E-2</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="1"/>
-        <v>5.5766666666666666E-2</v>
+        <v>0.24229999999999999</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
-        <v>0.90300000000000002</v>
+        <v>0.64733333333333343</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>0.94799999999999995</v>
+        <v>0.66800000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2093,19 +2093,19 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>94.797899999999998</v>
+        <v>62.445</v>
       </c>
       <c r="C17">
-        <v>6.7999999999999996E-3</v>
+        <v>7.7499999999999999E-2</v>
       </c>
       <c r="D17">
-        <v>5.5899999999999998E-2</v>
+        <v>0.2616</v>
       </c>
       <c r="E17">
-        <v>0.90300000000000002</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="F17">
-        <v>0.94799999999999995</v>
+        <v>0.624</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2113,19 +2113,19 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>94.737899999999996</v>
+        <v>68.047200000000004</v>
       </c>
       <c r="C18">
-        <v>7.0000000000000001E-3</v>
+        <v>6.5799999999999997E-2</v>
       </c>
       <c r="D18">
-        <v>5.6800000000000003E-2</v>
+        <v>0.23649999999999999</v>
       </c>
       <c r="E18">
-        <v>0.90200000000000002</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="F18">
-        <v>0.94699999999999995</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2133,19 +2133,19 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>94.878</v>
+        <v>69.968000000000004</v>
       </c>
       <c r="C19">
-        <v>6.7000000000000002E-3</v>
+        <v>6.2300000000000001E-2</v>
       </c>
       <c r="D19">
-        <v>5.4600000000000003E-2</v>
+        <v>0.2288</v>
       </c>
       <c r="E19">
-        <v>0.90400000000000003</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="F19">
-        <v>0.94899999999999995</v>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
@@ -2159,7 +2159,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="B2:F2"/>
+      <selection sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,8 +2531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>